<commit_message>
NIVEL FINAL - Attempt 1
</commit_message>
<xml_diff>
--- a/NIVEL FINAL/Attempt1/TitoJavierFranciscoMiguelGaldamez/Data/Config.xlsx
+++ b/NIVEL FINAL/Attempt1/TitoJavierFranciscoMiguelGaldamez/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\tito.miguel\repositorios\CertificationExam4\CollectWorkItems\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tito.miguel\repositorios\UiPath\NIVEL FINAL\Attempt1\TitoJavierFranciscoMiguelGaldamez\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="19200" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="19200" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,7 @@
     <t>https://acme-test.uipath.com</t>
   </si>
   <si>
-    <t>javier.galdamez@apptividad.com</t>
+    <t>ACME_Credential</t>
   </si>
 </sst>
 </file>
@@ -573,7 +573,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>